<commit_message>
More progress with performance management, diagrams for state management, blank project for state management, instruction pdfs for a number of tasks.
</commit_message>
<xml_diff>
--- a/08 - Spike - Performance Measurement/Spike 8 Data - Performance Measurement.xlsx
+++ b/08 - Spike - Performance Measurement/Spike 8 Data - Performance Measurement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam Huffer\Coding\COS30031 - 101633177\08 - Spike - Performance Measurement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E76AB8-B960-4D6C-8729-A32138CC44D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B763E5C-F037-4514-BC94-B83273DAFFE5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{A2983AF5-8AB3-4AAC-AC42-04C53262FF34}"/>
+    <workbookView xWindow="13305" yWindow="2085" windowWidth="21600" windowHeight="11385" xr2:uid="{A2983AF5-8AB3-4AAC-AC42-04C53262FF34}"/>
   </bookViews>
   <sheets>
     <sheet name="Single Tests" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="53">
   <si>
     <t>Linear Ramp-Up</t>
   </si>
@@ -183,6 +183,18 @@
   </si>
   <si>
     <t>Time (ns) / Item</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Multiple Methods</t>
+  </si>
+  <si>
+    <t>Single Method - Linear Ramp-Up</t>
+  </si>
+  <si>
+    <t>Single Method - Exponential Ramp-Up</t>
   </si>
 </sst>
 </file>
@@ -13491,12 +13503,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E58D08-7F09-4982-994F-1ABE6F9D317F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1.8681099999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3.7362800000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1.11001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4.4886500000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1.43658E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <f xml:space="preserve"> AVERAGE(B3:B7)</f>
+        <v>2.5279260000000005E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.97326199999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1.03434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1.75762</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>4</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.81033</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>5</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2.1109100000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="2">
+        <f xml:space="preserve"> AVERAGE(B12:B16)</f>
+        <v>1.5372924000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1.07172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.09883</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1.0057199999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.1382300000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>5</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1.2556099999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2">
+        <f xml:space="preserve"> AVERAGE(B21:B25)</f>
+        <v>1.1140219999999998</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -15098,7 +15304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53527B1E-66D6-47B3-BCE5-E2B18FDEFE56}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
@@ -15850,11 +16056,11 @@
         <v>3200</v>
       </c>
       <c r="E36" s="2">
-        <f xml:space="preserve"> C36/1000000000</f>
+        <f t="shared" ref="E36:E45" si="1" xml:space="preserve"> C36/1000000000</f>
         <v>3.1999999999999999E-6</v>
       </c>
       <c r="F36" s="2">
-        <f xml:space="preserve"> D36/1000000000</f>
+        <f t="shared" ref="F36:F45" si="2" xml:space="preserve"> D36/1000000000</f>
         <v>3.1999999999999999E-6</v>
       </c>
     </row>
@@ -15872,11 +16078,11 @@
         <v>9400</v>
       </c>
       <c r="E37" s="2">
-        <f xml:space="preserve"> C37/1000000000</f>
+        <f t="shared" si="1"/>
         <v>9.3999999999999998E-6</v>
       </c>
       <c r="F37" s="2">
-        <f xml:space="preserve"> D37/1000000000</f>
+        <f t="shared" si="2"/>
         <v>9.3999999999999998E-6</v>
       </c>
     </row>
@@ -15894,11 +16100,11 @@
         <v>3100</v>
       </c>
       <c r="E38" s="2">
-        <f xml:space="preserve"> C38/1000000000</f>
+        <f t="shared" si="1"/>
         <v>3.1E-6</v>
       </c>
       <c r="F38" s="2">
-        <f xml:space="preserve"> D38/1000000000</f>
+        <f t="shared" si="2"/>
         <v>3.1E-6</v>
       </c>
     </row>
@@ -15916,11 +16122,11 @@
         <v>3200</v>
       </c>
       <c r="E39" s="2">
-        <f xml:space="preserve"> C39/1000000000</f>
+        <f t="shared" si="1"/>
         <v>3.1999999999999999E-6</v>
       </c>
       <c r="F39" s="2">
-        <f xml:space="preserve"> D39/1000000000</f>
+        <f t="shared" si="2"/>
         <v>3.1999999999999999E-6</v>
       </c>
     </row>
@@ -15938,11 +16144,11 @@
         <v>3300</v>
       </c>
       <c r="E40" s="2">
-        <f xml:space="preserve"> C40/1000000000</f>
+        <f t="shared" si="1"/>
         <v>3.3000000000000002E-6</v>
       </c>
       <c r="F40" s="2">
-        <f xml:space="preserve"> D40/1000000000</f>
+        <f t="shared" si="2"/>
         <v>3.3000000000000002E-6</v>
       </c>
     </row>
@@ -15960,11 +16166,11 @@
         <v>440</v>
       </c>
       <c r="E41" s="2">
-        <f xml:space="preserve"> C41/1000000000</f>
+        <f t="shared" si="1"/>
         <v>4.4000000000000002E-6</v>
       </c>
       <c r="F41" s="2">
-        <f xml:space="preserve"> D41/1000000000</f>
+        <f t="shared" si="2"/>
         <v>4.4000000000000002E-7</v>
       </c>
     </row>
@@ -15982,11 +16188,11 @@
         <v>440</v>
       </c>
       <c r="E42" s="2">
-        <f xml:space="preserve"> C42/1000000000</f>
+        <f t="shared" si="1"/>
         <v>4.4000000000000002E-6</v>
       </c>
       <c r="F42" s="2">
-        <f xml:space="preserve"> D42/1000000000</f>
+        <f t="shared" si="2"/>
         <v>4.4000000000000002E-7</v>
       </c>
     </row>
@@ -16004,11 +16210,11 @@
         <v>450</v>
       </c>
       <c r="E43" s="2">
-        <f xml:space="preserve"> C43/1000000000</f>
+        <f t="shared" si="1"/>
         <v>4.5000000000000001E-6</v>
       </c>
       <c r="F43" s="2">
-        <f xml:space="preserve"> D43/1000000000</f>
+        <f t="shared" si="2"/>
         <v>4.4999999999999998E-7</v>
       </c>
     </row>
@@ -16026,11 +16232,11 @@
         <v>440</v>
       </c>
       <c r="E44" s="2">
-        <f xml:space="preserve"> C44/1000000000</f>
+        <f t="shared" si="1"/>
         <v>4.4000000000000002E-6</v>
       </c>
       <c r="F44" s="2">
-        <f xml:space="preserve"> D44/1000000000</f>
+        <f t="shared" si="2"/>
         <v>4.4000000000000002E-7</v>
       </c>
     </row>
@@ -16048,11 +16254,11 @@
         <v>530</v>
       </c>
       <c r="E45" s="2">
-        <f xml:space="preserve"> C45/1000000000</f>
+        <f t="shared" si="1"/>
         <v>5.3000000000000001E-6</v>
       </c>
       <c r="F45" s="2">
-        <f xml:space="preserve"> D45/1000000000</f>
+        <f t="shared" si="2"/>
         <v>5.3000000000000001E-7</v>
       </c>
     </row>
@@ -16070,11 +16276,11 @@
         <v>48</v>
       </c>
       <c r="E46" s="2">
-        <f t="shared" ref="E37:F65" si="1" xml:space="preserve"> C46/1000000000</f>
+        <f t="shared" ref="E46:F65" si="3" xml:space="preserve"> C46/1000000000</f>
         <v>4.7999999999999998E-6</v>
       </c>
       <c r="F46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.8E-8</v>
       </c>
     </row>
@@ -16092,11 +16298,11 @@
         <v>52</v>
       </c>
       <c r="E47" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.2000000000000002E-6</v>
       </c>
       <c r="F47" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.2000000000000002E-8</v>
       </c>
     </row>
@@ -16114,11 +16320,11 @@
         <v>51</v>
       </c>
       <c r="E48" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.1000000000000003E-6</v>
       </c>
       <c r="F48" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.1E-8</v>
       </c>
     </row>
@@ -16136,11 +16342,11 @@
         <v>46</v>
       </c>
       <c r="E49" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.6E-6</v>
       </c>
       <c r="F49" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.6000000000000002E-8</v>
       </c>
     </row>
@@ -16158,11 +16364,11 @@
         <v>48</v>
       </c>
       <c r="E50" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.7999999999999998E-6</v>
       </c>
       <c r="F50" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.8E-8</v>
       </c>
     </row>
@@ -16180,11 +16386,11 @@
         <v>86</v>
       </c>
       <c r="E51" s="2">
-        <f xml:space="preserve"> C51/1000000000</f>
+        <f t="shared" ref="E51:E60" si="4" xml:space="preserve"> C51/1000000000</f>
         <v>8.6000000000000003E-5</v>
       </c>
       <c r="F51" s="2">
-        <f xml:space="preserve"> D51/1000000000</f>
+        <f t="shared" si="3"/>
         <v>8.6000000000000002E-8</v>
       </c>
     </row>
@@ -16202,11 +16408,11 @@
         <v>29</v>
       </c>
       <c r="E52" s="2">
-        <f xml:space="preserve"> C52/1000000000</f>
+        <f t="shared" si="3"/>
         <v>2.9099999999999999E-5</v>
       </c>
       <c r="F52" s="2">
-        <f xml:space="preserve"> D52/1000000000</f>
+        <f t="shared" si="3"/>
         <v>2.9000000000000002E-8</v>
       </c>
     </row>
@@ -16224,11 +16430,11 @@
         <v>34</v>
       </c>
       <c r="E53" s="2">
-        <f xml:space="preserve"> C53/1000000000</f>
+        <f t="shared" si="3"/>
         <v>3.4100000000000002E-5</v>
       </c>
       <c r="F53" s="2">
-        <f xml:space="preserve"> D53/1000000000</f>
+        <f t="shared" si="3"/>
         <v>3.4E-8</v>
       </c>
     </row>
@@ -16246,11 +16452,11 @@
         <v>35</v>
       </c>
       <c r="E54" s="2">
-        <f xml:space="preserve"> C54/1000000000</f>
+        <f t="shared" si="3"/>
         <v>3.5599999999999998E-5</v>
       </c>
       <c r="F54" s="2">
-        <f xml:space="preserve"> D54/1000000000</f>
+        <f t="shared" si="3"/>
         <v>3.5000000000000002E-8</v>
       </c>
     </row>
@@ -16268,11 +16474,11 @@
         <v>28</v>
       </c>
       <c r="E55" s="2">
-        <f xml:space="preserve"> C55/1000000000</f>
+        <f t="shared" si="3"/>
         <v>2.8900000000000001E-5</v>
       </c>
       <c r="F55" s="2">
-        <f xml:space="preserve"> D55/1000000000</f>
+        <f t="shared" si="3"/>
         <v>2.7999999999999999E-8</v>
       </c>
     </row>
@@ -16290,11 +16496,11 @@
         <v>10</v>
       </c>
       <c r="E56">
-        <f xml:space="preserve"> C56/1000000000</f>
+        <f t="shared" si="3"/>
         <v>1.071E-4</v>
       </c>
       <c r="F56" s="2">
-        <f xml:space="preserve"> D56/1000000000</f>
+        <f t="shared" si="3"/>
         <v>1E-8</v>
       </c>
     </row>
@@ -16312,11 +16518,11 @@
         <v>15</v>
       </c>
       <c r="E57" s="2">
-        <f xml:space="preserve"> C57/1000000000</f>
+        <f t="shared" si="3"/>
         <v>1.5410000000000001E-4</v>
       </c>
       <c r="F57" s="2">
-        <f xml:space="preserve"> D57/1000000000</f>
+        <f t="shared" si="3"/>
         <v>1.4999999999999999E-8</v>
       </c>
     </row>
@@ -16334,11 +16540,11 @@
         <v>14</v>
       </c>
       <c r="E58" s="2">
-        <f xml:space="preserve"> C58/1000000000</f>
+        <f t="shared" si="3"/>
         <v>1.4410000000000001E-4</v>
       </c>
       <c r="F58" s="2">
-        <f xml:space="preserve"> D58/1000000000</f>
+        <f t="shared" si="3"/>
         <v>1.4E-8</v>
       </c>
     </row>
@@ -16356,11 +16562,11 @@
         <v>15</v>
       </c>
       <c r="E59" s="2">
-        <f xml:space="preserve"> C59/1000000000</f>
+        <f t="shared" si="3"/>
         <v>1.5029999999999999E-4</v>
       </c>
       <c r="F59" s="2">
-        <f xml:space="preserve"> D59/1000000000</f>
+        <f t="shared" si="3"/>
         <v>1.4999999999999999E-8</v>
       </c>
     </row>
@@ -16378,11 +16584,11 @@
         <v>12</v>
       </c>
       <c r="E60" s="2">
-        <f xml:space="preserve"> C60/1000000000</f>
+        <f t="shared" si="3"/>
         <v>1.2439999999999999E-4</v>
       </c>
       <c r="F60" s="2">
-        <f xml:space="preserve"> D60/1000000000</f>
+        <f t="shared" si="3"/>
         <v>1.2E-8</v>
       </c>
     </row>
@@ -16402,11 +16608,11 @@
         <v>4440</v>
       </c>
       <c r="E61" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.4399999999999998E-6</v>
       </c>
       <c r="F61" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.4399999999999998E-6</v>
       </c>
     </row>
@@ -16426,11 +16632,11 @@
         <v>460</v>
       </c>
       <c r="E62" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.6E-6</v>
       </c>
       <c r="F62" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.5999999999999999E-7</v>
       </c>
     </row>
@@ -16450,11 +16656,11 @@
         <v>56.6</v>
       </c>
       <c r="E63" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.1140000000000001E-5</v>
       </c>
       <c r="F63" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.6600000000000004E-8</v>
       </c>
     </row>
@@ -16474,11 +16680,11 @@
         <v>42.4</v>
       </c>
       <c r="E64" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.2740000000000001E-5</v>
       </c>
       <c r="F64" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.2399999999999996E-8</v>
       </c>
     </row>
@@ -16498,11 +16704,11 @@
         <v>13.2</v>
       </c>
       <c r="E65" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.36E-4</v>
       </c>
       <c r="F65" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3199999999999999E-8</v>
       </c>
     </row>

</xml_diff>